<commit_message>
added menu save files, improved performance
</commit_message>
<xml_diff>
--- a/tests/test1/Schema di funzionamento_rev1.1_bom_revised_updated.xlsx
+++ b/tests/test1/Schema di funzionamento_rev1.1_bom_revised_updated.xlsx
@@ -37,7 +37,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
@@ -116,8 +116,15 @@
       <sz val="11"/>
       <u val="single"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -140,6 +147,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00CCCCCC"/>
         <bgColor rgb="00CCCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00800080"/>
+        <bgColor rgb="00800080"/>
       </patternFill>
     </fill>
   </fills>
@@ -192,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -271,6 +284,7 @@
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -309,6 +323,12 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -592,10 +612,10 @@
   <dimension ref="A1:AH662"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A26" sqref="A26:XFD26"/>
+      <selection pane="bottomRight" activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2026,56 +2046,56 @@
       <c r="AH23" s="13" t="n"/>
     </row>
     <row r="24" ht="14.4" customHeight="1">
-      <c r="A24" s="28" t="n">
+      <c r="A24" s="29" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="28" t="inlineStr">
+      <c r="B24" s="29" t="inlineStr">
         <is>
           <t>LS</t>
         </is>
       </c>
-      <c r="C24" s="28" t="n">
+      <c r="C24" s="29" t="n">
         <v>202</v>
       </c>
-      <c r="D24" s="28" t="n"/>
-      <c r="E24" s="29" t="inlineStr">
+      <c r="D24" s="29" t="n"/>
+      <c r="E24" s="30" t="inlineStr">
         <is>
           <t>LS202</t>
         </is>
       </c>
-      <c r="F24" s="28" t="n"/>
-      <c r="G24" s="30" t="n"/>
-      <c r="H24" s="28" t="n"/>
-      <c r="I24" s="28" t="n"/>
-      <c r="J24" s="28" t="n"/>
-      <c r="K24" s="28" t="n"/>
-      <c r="L24" s="28" t="n"/>
-      <c r="M24" s="31" t="inlineStr">
+      <c r="F24" s="29" t="n"/>
+      <c r="G24" s="31" t="n"/>
+      <c r="H24" s="29" t="n"/>
+      <c r="I24" s="29" t="n"/>
+      <c r="J24" s="29" t="n"/>
+      <c r="K24" s="29" t="n"/>
+      <c r="L24" s="29" t="n"/>
+      <c r="M24" s="32" t="inlineStr">
         <is>
           <t>Livellostato</t>
         </is>
       </c>
-      <c r="N24" s="31" t="n"/>
-      <c r="O24" s="28" t="n"/>
-      <c r="P24" s="31" t="n"/>
-      <c r="Q24" s="32" t="n"/>
-      <c r="R24" s="28" t="n"/>
-      <c r="S24" s="28" t="n"/>
-      <c r="T24" s="28" t="n"/>
-      <c r="U24" s="28" t="n"/>
-      <c r="V24" s="28" t="n"/>
-      <c r="W24" s="28" t="n"/>
-      <c r="X24" s="31" t="n"/>
-      <c r="Y24" s="31" t="n"/>
-      <c r="Z24" s="33" t="n"/>
-      <c r="AA24" s="31" t="n"/>
-      <c r="AB24" s="28" t="n"/>
-      <c r="AC24" s="28" t="n"/>
-      <c r="AD24" s="31" t="n"/>
-      <c r="AE24" s="31" t="n"/>
-      <c r="AF24" s="31" t="n"/>
-      <c r="AG24" s="28" t="n"/>
-      <c r="AH24" s="34" t="n"/>
+      <c r="N24" s="32" t="n"/>
+      <c r="O24" s="29" t="n"/>
+      <c r="P24" s="32" t="n"/>
+      <c r="Q24" s="33" t="n"/>
+      <c r="R24" s="29" t="n"/>
+      <c r="S24" s="29" t="n"/>
+      <c r="T24" s="29" t="n"/>
+      <c r="U24" s="29" t="n"/>
+      <c r="V24" s="29" t="n"/>
+      <c r="W24" s="29" t="n"/>
+      <c r="X24" s="32" t="n"/>
+      <c r="Y24" s="32" t="n"/>
+      <c r="Z24" s="34" t="n"/>
+      <c r="AA24" s="32" t="n"/>
+      <c r="AB24" s="29" t="n"/>
+      <c r="AC24" s="29" t="n"/>
+      <c r="AD24" s="32" t="n"/>
+      <c r="AE24" s="32" t="n"/>
+      <c r="AF24" s="32" t="n"/>
+      <c r="AG24" s="29" t="n"/>
+      <c r="AH24" s="35" t="n"/>
     </row>
     <row r="25" ht="14.4" customHeight="1">
       <c r="A25" s="8" t="n">
@@ -2132,58 +2152,58 @@
       <c r="AH25" s="13" t="n"/>
     </row>
     <row r="26" ht="14.4" customFormat="1" customHeight="1" s="21">
-      <c r="A26" s="35" t="n">
+      <c r="A26" s="36" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="35" t="inlineStr">
+      <c r="B26" s="36" t="inlineStr">
         <is>
           <t>LS</t>
         </is>
       </c>
-      <c r="C26" s="35" t="inlineStr">
+      <c r="C26" s="36" t="inlineStr">
         <is>
           <t>701</t>
         </is>
       </c>
-      <c r="D26" s="35" t="inlineStr"/>
-      <c r="E26" s="36" t="inlineStr">
+      <c r="D26" s="36" t="inlineStr"/>
+      <c r="E26" s="37" t="inlineStr">
         <is>
           <t>LS701</t>
         </is>
       </c>
-      <c r="F26" s="35" t="inlineStr"/>
-      <c r="G26" s="35" t="inlineStr"/>
-      <c r="H26" s="35" t="inlineStr"/>
-      <c r="I26" s="35" t="inlineStr"/>
-      <c r="J26" s="35" t="inlineStr"/>
-      <c r="K26" s="35" t="inlineStr"/>
-      <c r="L26" s="35" t="inlineStr"/>
-      <c r="M26" s="37" t="inlineStr">
+      <c r="F26" s="36" t="inlineStr"/>
+      <c r="G26" s="36" t="inlineStr"/>
+      <c r="H26" s="36" t="inlineStr"/>
+      <c r="I26" s="36" t="inlineStr"/>
+      <c r="J26" s="36" t="inlineStr"/>
+      <c r="K26" s="36" t="inlineStr"/>
+      <c r="L26" s="36" t="inlineStr"/>
+      <c r="M26" s="38" t="inlineStr">
         <is>
           <t>Livellostato</t>
         </is>
       </c>
-      <c r="N26" s="37" t="n"/>
-      <c r="O26" s="35" t="inlineStr"/>
-      <c r="P26" s="37" t="inlineStr"/>
-      <c r="Q26" s="38" t="inlineStr"/>
-      <c r="R26" s="35" t="inlineStr"/>
-      <c r="S26" s="35" t="inlineStr"/>
-      <c r="T26" s="35" t="inlineStr"/>
-      <c r="U26" s="35" t="n"/>
-      <c r="V26" s="35" t="inlineStr"/>
-      <c r="W26" s="35" t="inlineStr"/>
-      <c r="X26" s="37" t="inlineStr"/>
-      <c r="Y26" s="37" t="inlineStr"/>
-      <c r="Z26" s="39" t="inlineStr"/>
-      <c r="AA26" s="37" t="inlineStr"/>
-      <c r="AB26" s="35" t="inlineStr"/>
-      <c r="AC26" s="35" t="inlineStr"/>
-      <c r="AD26" s="37" t="inlineStr"/>
-      <c r="AE26" s="37" t="inlineStr"/>
-      <c r="AF26" s="37" t="inlineStr"/>
-      <c r="AG26" s="35" t="inlineStr"/>
-      <c r="AH26" s="40" t="inlineStr"/>
+      <c r="N26" s="38" t="n"/>
+      <c r="O26" s="36" t="inlineStr"/>
+      <c r="P26" s="38" t="inlineStr"/>
+      <c r="Q26" s="39" t="inlineStr"/>
+      <c r="R26" s="36" t="inlineStr"/>
+      <c r="S26" s="36" t="inlineStr"/>
+      <c r="T26" s="36" t="inlineStr"/>
+      <c r="U26" s="36" t="n"/>
+      <c r="V26" s="36" t="inlineStr"/>
+      <c r="W26" s="36" t="inlineStr"/>
+      <c r="X26" s="38" t="inlineStr"/>
+      <c r="Y26" s="38" t="inlineStr"/>
+      <c r="Z26" s="40" t="inlineStr"/>
+      <c r="AA26" s="38" t="inlineStr"/>
+      <c r="AB26" s="36" t="inlineStr"/>
+      <c r="AC26" s="36" t="inlineStr"/>
+      <c r="AD26" s="38" t="inlineStr"/>
+      <c r="AE26" s="38" t="inlineStr"/>
+      <c r="AF26" s="38" t="inlineStr"/>
+      <c r="AG26" s="36" t="inlineStr"/>
+      <c r="AH26" s="41" t="inlineStr"/>
     </row>
     <row r="27" ht="14.4" customHeight="1">
       <c r="A27" s="8" t="n">
@@ -2835,64 +2855,76 @@
       <c r="AG38" s="8" t="n"/>
       <c r="AH38" s="13" t="n"/>
     </row>
-    <row r="39" ht="14.4" customHeight="1">
-      <c r="A39" s="8" t="n">
+    <row r="39" ht="14.4" customFormat="1" customHeight="1" s="28">
+      <c r="A39" s="16" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="8" t="inlineStr">
+      <c r="B39" s="16" t="inlineStr">
         <is>
           <t>XV</t>
         </is>
       </c>
-      <c r="C39" s="8" t="n">
+      <c r="C39" s="16" t="n">
         <v>851</v>
       </c>
-      <c r="D39" s="8" t="n"/>
-      <c r="E39" s="12" t="inlineStr">
+      <c r="D39" s="16" t="n"/>
+      <c r="E39" s="42" t="inlineStr">
         <is>
           <t>XV851</t>
         </is>
       </c>
-      <c r="F39" s="8" t="n"/>
-      <c r="G39" s="8" t="n"/>
-      <c r="H39" s="8" t="n"/>
-      <c r="I39" s="8" t="n"/>
-      <c r="J39" s="8" t="n"/>
-      <c r="K39" s="8" t="n"/>
-      <c r="L39" s="8" t="n"/>
-      <c r="M39" s="9" t="inlineStr">
+      <c r="F39" s="16" t="n"/>
+      <c r="G39" s="16" t="n"/>
+      <c r="H39" s="16" t="n"/>
+      <c r="I39" s="16" t="n"/>
+      <c r="J39" s="16" t="n"/>
+      <c r="K39" s="16" t="n"/>
+      <c r="L39" s="16" t="n"/>
+      <c r="M39" s="18" t="inlineStr">
         <is>
           <t>Ball Valve with Pneumatic actuator</t>
         </is>
       </c>
-      <c r="N39" s="9" t="n"/>
-      <c r="O39" s="8" t="n"/>
-      <c r="P39" s="9" t="n"/>
-      <c r="Q39" s="10" t="n"/>
-      <c r="R39" s="8" t="n"/>
-      <c r="S39" s="8" t="n"/>
-      <c r="T39" s="8" t="n"/>
-      <c r="U39" s="8" t="n"/>
-      <c r="V39" s="8" t="n"/>
-      <c r="W39" s="8" t="n"/>
-      <c r="X39" s="9" t="n"/>
-      <c r="Y39" s="9" t="n"/>
-      <c r="Z39" s="11" t="n"/>
-      <c r="AA39" s="9" t="n"/>
-      <c r="AB39" s="8" t="n"/>
-      <c r="AC39" s="8" t="n"/>
-      <c r="AD39" s="9" t="n"/>
-      <c r="AE39" s="9" t="n"/>
-      <c r="AF39" s="9" t="n"/>
-      <c r="AG39" s="8" t="n"/>
-      <c r="AH39" s="13" t="n"/>
+      <c r="N39" s="18" t="n"/>
+      <c r="O39" s="16" t="n"/>
+      <c r="P39" s="18" t="n"/>
+      <c r="Q39" s="19" t="n"/>
+      <c r="R39" s="16" t="n"/>
+      <c r="S39" s="16" t="n"/>
+      <c r="T39" s="16" t="n"/>
+      <c r="U39" s="16" t="n"/>
+      <c r="V39" s="16" t="n"/>
+      <c r="W39" s="16" t="n"/>
+      <c r="X39" s="18" t="n"/>
+      <c r="Y39" s="18" t="n"/>
+      <c r="Z39" s="17" t="n"/>
+      <c r="AA39" s="18" t="n"/>
+      <c r="AB39" s="16" t="n"/>
+      <c r="AC39" s="16" t="n"/>
+      <c r="AD39" s="18" t="n"/>
+      <c r="AE39" s="18" t="n"/>
+      <c r="AF39" s="18" t="n"/>
+      <c r="AG39" s="16" t="n"/>
+      <c r="AH39" s="20" t="n"/>
     </row>
     <row r="40" ht="14.4" customHeight="1">
-      <c r="A40" s="8" t="n"/>
-      <c r="B40" s="8" t="n"/>
-      <c r="C40" s="8" t="n"/>
+      <c r="A40" s="8" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="8" t="inlineStr">
+        <is>
+          <t>XV</t>
+        </is>
+      </c>
+      <c r="C40" s="8" t="n">
+        <v>851</v>
+      </c>
       <c r="D40" s="8" t="n"/>
-      <c r="E40" s="12" t="n"/>
+      <c r="E40" s="43" t="inlineStr">
+        <is>
+          <t>XV851</t>
+        </is>
+      </c>
       <c r="F40" s="8" t="n"/>
       <c r="G40" s="8" t="n"/>
       <c r="H40" s="8" t="n"/>
@@ -2900,7 +2932,11 @@
       <c r="J40" s="8" t="n"/>
       <c r="K40" s="8" t="n"/>
       <c r="L40" s="8" t="n"/>
-      <c r="M40" s="9" t="n"/>
+      <c r="M40" s="9" t="inlineStr">
+        <is>
+          <t>Ball Valve with Pneumatic actuator</t>
+        </is>
+      </c>
       <c r="N40" s="9" t="n"/>
       <c r="O40" s="8" t="n"/>
       <c r="P40" s="9" t="n"/>

</xml_diff>

<commit_message>
changements in XLS table are reflected in exported xls file
</commit_message>
<xml_diff>
--- a/tests/test1/Schema di funzionamento_rev1.1_bom_revised_updated.xlsx
+++ b/tests/test1/Schema di funzionamento_rev1.1_bom_revised_updated.xlsx
@@ -124,7 +124,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -147,12 +147,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="00CCCCCC"/>
         <bgColor rgb="00CCCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00800080"/>
-        <bgColor rgb="00800080"/>
       </patternFill>
     </fill>
   </fills>
@@ -205,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -323,12 +317,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2054,48 +2042,50 @@
           <t>LS</t>
         </is>
       </c>
-      <c r="C24" s="29" t="n">
-        <v>202</v>
+      <c r="C24" s="29" t="inlineStr">
+        <is>
+          <t>203</t>
+        </is>
       </c>
-      <c r="D24" s="29" t="n"/>
+      <c r="D24" s="29" t="inlineStr"/>
       <c r="E24" s="30" t="inlineStr">
         <is>
-          <t>LS202</t>
+          <t>LS203</t>
         </is>
       </c>
-      <c r="F24" s="29" t="n"/>
-      <c r="G24" s="31" t="n"/>
-      <c r="H24" s="29" t="n"/>
-      <c r="I24" s="29" t="n"/>
-      <c r="J24" s="29" t="n"/>
-      <c r="K24" s="29" t="n"/>
-      <c r="L24" s="29" t="n"/>
+      <c r="F24" s="29" t="inlineStr"/>
+      <c r="G24" s="31" t="inlineStr"/>
+      <c r="H24" s="29" t="inlineStr"/>
+      <c r="I24" s="29" t="inlineStr"/>
+      <c r="J24" s="29" t="inlineStr"/>
+      <c r="K24" s="29" t="inlineStr"/>
+      <c r="L24" s="29" t="inlineStr"/>
       <c r="M24" s="32" t="inlineStr">
         <is>
           <t>Livellostato</t>
         </is>
       </c>
-      <c r="N24" s="32" t="n"/>
-      <c r="O24" s="29" t="n"/>
-      <c r="P24" s="32" t="n"/>
-      <c r="Q24" s="33" t="n"/>
-      <c r="R24" s="29" t="n"/>
-      <c r="S24" s="29" t="n"/>
-      <c r="T24" s="29" t="n"/>
-      <c r="U24" s="29" t="n"/>
-      <c r="V24" s="29" t="n"/>
-      <c r="W24" s="29" t="n"/>
-      <c r="X24" s="32" t="n"/>
-      <c r="Y24" s="32" t="n"/>
-      <c r="Z24" s="34" t="n"/>
-      <c r="AA24" s="32" t="n"/>
-      <c r="AB24" s="29" t="n"/>
-      <c r="AC24" s="29" t="n"/>
-      <c r="AD24" s="32" t="n"/>
-      <c r="AE24" s="32" t="n"/>
-      <c r="AF24" s="32" t="n"/>
-      <c r="AG24" s="29" t="n"/>
-      <c r="AH24" s="35" t="n"/>
+      <c r="N24" s="32" t="inlineStr"/>
+      <c r="O24" s="29" t="inlineStr"/>
+      <c r="P24" s="32" t="inlineStr"/>
+      <c r="Q24" s="33" t="inlineStr"/>
+      <c r="R24" s="29" t="inlineStr"/>
+      <c r="S24" s="29" t="inlineStr"/>
+      <c r="T24" s="29" t="inlineStr"/>
+      <c r="U24" s="29" t="inlineStr"/>
+      <c r="V24" s="29" t="inlineStr"/>
+      <c r="W24" s="29" t="inlineStr"/>
+      <c r="X24" s="32" t="inlineStr"/>
+      <c r="Y24" s="32" t="inlineStr"/>
+      <c r="Z24" s="34" t="inlineStr"/>
+      <c r="AA24" s="32" t="inlineStr"/>
+      <c r="AB24" s="29" t="inlineStr"/>
+      <c r="AC24" s="29" t="inlineStr"/>
+      <c r="AD24" s="32" t="inlineStr"/>
+      <c r="AE24" s="32" t="inlineStr"/>
+      <c r="AF24" s="32" t="inlineStr"/>
+      <c r="AG24" s="29" t="inlineStr"/>
+      <c r="AH24" s="35" t="inlineStr"/>
     </row>
     <row r="25" ht="14.4" customHeight="1">
       <c r="A25" s="8" t="n">
@@ -2183,14 +2173,14 @@
           <t>Livellostato</t>
         </is>
       </c>
-      <c r="N26" s="38" t="n"/>
+      <c r="N26" s="38" t="inlineStr"/>
       <c r="O26" s="36" t="inlineStr"/>
       <c r="P26" s="38" t="inlineStr"/>
       <c r="Q26" s="39" t="inlineStr"/>
       <c r="R26" s="36" t="inlineStr"/>
       <c r="S26" s="36" t="inlineStr"/>
       <c r="T26" s="36" t="inlineStr"/>
-      <c r="U26" s="36" t="n"/>
+      <c r="U26" s="36" t="inlineStr"/>
       <c r="V26" s="36" t="inlineStr"/>
       <c r="W26" s="36" t="inlineStr"/>
       <c r="X26" s="38" t="inlineStr"/>
@@ -2868,7 +2858,7 @@
         <v>851</v>
       </c>
       <c r="D39" s="16" t="n"/>
-      <c r="E39" s="42" t="inlineStr">
+      <c r="E39" s="27" t="inlineStr">
         <is>
           <t>XV851</t>
         </is>
@@ -2908,56 +2898,58 @@
       <c r="AH39" s="20" t="n"/>
     </row>
     <row r="40" ht="14.4" customHeight="1">
-      <c r="A40" s="8" t="n">
+      <c r="A40" s="29" t="n">
         <v>39</v>
       </c>
-      <c r="B40" s="8" t="inlineStr">
+      <c r="B40" s="29" t="inlineStr">
         <is>
           <t>XV</t>
         </is>
       </c>
-      <c r="C40" s="8" t="n">
-        <v>851</v>
-      </c>
-      <c r="D40" s="8" t="n"/>
-      <c r="E40" s="43" t="inlineStr">
+      <c r="C40" s="29" t="inlineStr">
         <is>
-          <t>XV851</t>
+          <t>852</t>
         </is>
       </c>
-      <c r="F40" s="8" t="n"/>
-      <c r="G40" s="8" t="n"/>
-      <c r="H40" s="8" t="n"/>
-      <c r="I40" s="8" t="n"/>
-      <c r="J40" s="8" t="n"/>
-      <c r="K40" s="8" t="n"/>
-      <c r="L40" s="8" t="n"/>
-      <c r="M40" s="9" t="inlineStr">
+      <c r="D40" s="29" t="inlineStr"/>
+      <c r="E40" s="30" t="inlineStr">
+        <is>
+          <t>XV852</t>
+        </is>
+      </c>
+      <c r="F40" s="29" t="inlineStr"/>
+      <c r="G40" s="29" t="inlineStr"/>
+      <c r="H40" s="29" t="inlineStr"/>
+      <c r="I40" s="29" t="inlineStr"/>
+      <c r="J40" s="29" t="inlineStr"/>
+      <c r="K40" s="29" t="inlineStr"/>
+      <c r="L40" s="29" t="inlineStr"/>
+      <c r="M40" s="32" t="inlineStr">
         <is>
           <t>Ball Valve with Pneumatic actuator</t>
         </is>
       </c>
-      <c r="N40" s="9" t="n"/>
-      <c r="O40" s="8" t="n"/>
-      <c r="P40" s="9" t="n"/>
-      <c r="Q40" s="10" t="n"/>
-      <c r="R40" s="8" t="n"/>
-      <c r="S40" s="8" t="n"/>
-      <c r="T40" s="8" t="n"/>
-      <c r="U40" s="8" t="n"/>
-      <c r="V40" s="8" t="n"/>
-      <c r="W40" s="8" t="n"/>
-      <c r="X40" s="9" t="n"/>
-      <c r="Y40" s="9" t="n"/>
-      <c r="Z40" s="11" t="n"/>
-      <c r="AA40" s="9" t="n"/>
-      <c r="AB40" s="8" t="n"/>
-      <c r="AC40" s="8" t="n"/>
-      <c r="AD40" s="9" t="n"/>
-      <c r="AE40" s="9" t="n"/>
-      <c r="AF40" s="9" t="n"/>
-      <c r="AG40" s="8" t="n"/>
-      <c r="AH40" s="13" t="n"/>
+      <c r="N40" s="32" t="inlineStr"/>
+      <c r="O40" s="29" t="inlineStr"/>
+      <c r="P40" s="32" t="inlineStr"/>
+      <c r="Q40" s="33" t="inlineStr"/>
+      <c r="R40" s="29" t="inlineStr"/>
+      <c r="S40" s="29" t="inlineStr"/>
+      <c r="T40" s="29" t="inlineStr"/>
+      <c r="U40" s="29" t="inlineStr"/>
+      <c r="V40" s="29" t="inlineStr"/>
+      <c r="W40" s="29" t="inlineStr"/>
+      <c r="X40" s="32" t="inlineStr"/>
+      <c r="Y40" s="32" t="inlineStr"/>
+      <c r="Z40" s="34" t="inlineStr"/>
+      <c r="AA40" s="32" t="inlineStr"/>
+      <c r="AB40" s="29" t="inlineStr"/>
+      <c r="AC40" s="29" t="inlineStr"/>
+      <c r="AD40" s="32" t="inlineStr"/>
+      <c r="AE40" s="32" t="inlineStr"/>
+      <c r="AF40" s="32" t="inlineStr"/>
+      <c r="AG40" s="29" t="inlineStr"/>
+      <c r="AH40" s="35" t="inlineStr"/>
     </row>
     <row r="41" ht="14.4" customHeight="1">
       <c r="A41" s="8" t="n"/>

</xml_diff>

<commit_message>
ver:2.4, import xls->dxf overwrite table dxf + warning for user
</commit_message>
<xml_diff>
--- a/tests/test1/Schema di funzionamento_rev1.1_bom_revised_updated.xlsx
+++ b/tests/test1/Schema di funzionamento_rev1.1_bom_revised_updated.xlsx
@@ -199,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -279,27 +279,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -316,6 +295,24 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2034,58 +2031,56 @@
       <c r="AH23" s="13" t="n"/>
     </row>
     <row r="24" ht="14.4" customHeight="1">
-      <c r="A24" s="29" t="n">
+      <c r="A24" s="8" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="29" t="inlineStr">
+      <c r="B24" s="8" t="inlineStr">
         <is>
           <t>LS</t>
         </is>
       </c>
-      <c r="C24" s="29" t="inlineStr">
+      <c r="C24" s="8" t="n">
+        <v>202</v>
+      </c>
+      <c r="D24" s="8" t="n"/>
+      <c r="E24" s="12" t="inlineStr">
         <is>
-          <t>203</t>
+          <t>LS202</t>
         </is>
       </c>
-      <c r="D24" s="29" t="inlineStr"/>
-      <c r="E24" s="30" t="inlineStr">
-        <is>
-          <t>LS203</t>
-        </is>
-      </c>
-      <c r="F24" s="29" t="inlineStr"/>
-      <c r="G24" s="31" t="inlineStr"/>
-      <c r="H24" s="29" t="inlineStr"/>
-      <c r="I24" s="29" t="inlineStr"/>
-      <c r="J24" s="29" t="inlineStr"/>
-      <c r="K24" s="29" t="inlineStr"/>
-      <c r="L24" s="29" t="inlineStr"/>
-      <c r="M24" s="32" t="inlineStr">
+      <c r="F24" s="8" t="n"/>
+      <c r="G24" s="16" t="n"/>
+      <c r="H24" s="8" t="n"/>
+      <c r="I24" s="8" t="n"/>
+      <c r="J24" s="8" t="n"/>
+      <c r="K24" s="8" t="n"/>
+      <c r="L24" s="8" t="n"/>
+      <c r="M24" s="9" t="inlineStr">
         <is>
           <t>Livellostato</t>
         </is>
       </c>
-      <c r="N24" s="32" t="inlineStr"/>
-      <c r="O24" s="29" t="inlineStr"/>
-      <c r="P24" s="32" t="inlineStr"/>
-      <c r="Q24" s="33" t="inlineStr"/>
-      <c r="R24" s="29" t="inlineStr"/>
-      <c r="S24" s="29" t="inlineStr"/>
-      <c r="T24" s="29" t="inlineStr"/>
-      <c r="U24" s="29" t="inlineStr"/>
-      <c r="V24" s="29" t="inlineStr"/>
-      <c r="W24" s="29" t="inlineStr"/>
-      <c r="X24" s="32" t="inlineStr"/>
-      <c r="Y24" s="32" t="inlineStr"/>
-      <c r="Z24" s="34" t="inlineStr"/>
-      <c r="AA24" s="32" t="inlineStr"/>
-      <c r="AB24" s="29" t="inlineStr"/>
-      <c r="AC24" s="29" t="inlineStr"/>
-      <c r="AD24" s="32" t="inlineStr"/>
-      <c r="AE24" s="32" t="inlineStr"/>
-      <c r="AF24" s="32" t="inlineStr"/>
-      <c r="AG24" s="29" t="inlineStr"/>
-      <c r="AH24" s="35" t="inlineStr"/>
+      <c r="N24" s="9" t="n"/>
+      <c r="O24" s="8" t="n"/>
+      <c r="P24" s="9" t="n"/>
+      <c r="Q24" s="10" t="n"/>
+      <c r="R24" s="8" t="n"/>
+      <c r="S24" s="8" t="n"/>
+      <c r="T24" s="8" t="n"/>
+      <c r="U24" s="8" t="n"/>
+      <c r="V24" s="8" t="n"/>
+      <c r="W24" s="8" t="n"/>
+      <c r="X24" s="9" t="n"/>
+      <c r="Y24" s="9" t="n"/>
+      <c r="Z24" s="11" t="n"/>
+      <c r="AA24" s="9" t="n"/>
+      <c r="AB24" s="8" t="n"/>
+      <c r="AC24" s="8" t="n"/>
+      <c r="AD24" s="9" t="n"/>
+      <c r="AE24" s="9" t="n"/>
+      <c r="AF24" s="9" t="n"/>
+      <c r="AG24" s="8" t="n"/>
+      <c r="AH24" s="13" t="n"/>
     </row>
     <row r="25" ht="14.4" customHeight="1">
       <c r="A25" s="8" t="n">
@@ -2142,58 +2137,58 @@
       <c r="AH25" s="13" t="n"/>
     </row>
     <row r="26" ht="14.4" customFormat="1" customHeight="1" s="21">
-      <c r="A26" s="36" t="n">
+      <c r="A26" s="29" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="36" t="inlineStr">
+      <c r="B26" s="29" t="inlineStr">
         <is>
           <t>LS</t>
         </is>
       </c>
-      <c r="C26" s="36" t="inlineStr">
+      <c r="C26" s="29" t="inlineStr">
         <is>
-          <t>701</t>
+          <t>506</t>
         </is>
       </c>
-      <c r="D26" s="36" t="inlineStr"/>
-      <c r="E26" s="37" t="inlineStr">
+      <c r="D26" s="29" t="inlineStr"/>
+      <c r="E26" s="30" t="inlineStr">
         <is>
-          <t>LS701</t>
+          <t>LS506</t>
         </is>
       </c>
-      <c r="F26" s="36" t="inlineStr"/>
-      <c r="G26" s="36" t="inlineStr"/>
-      <c r="H26" s="36" t="inlineStr"/>
-      <c r="I26" s="36" t="inlineStr"/>
-      <c r="J26" s="36" t="inlineStr"/>
-      <c r="K26" s="36" t="inlineStr"/>
-      <c r="L26" s="36" t="inlineStr"/>
-      <c r="M26" s="38" t="inlineStr">
+      <c r="F26" s="29" t="inlineStr"/>
+      <c r="G26" s="29" t="inlineStr"/>
+      <c r="H26" s="29" t="inlineStr"/>
+      <c r="I26" s="29" t="inlineStr"/>
+      <c r="J26" s="29" t="inlineStr"/>
+      <c r="K26" s="29" t="inlineStr"/>
+      <c r="L26" s="29" t="inlineStr"/>
+      <c r="M26" s="31" t="inlineStr">
         <is>
           <t>Livellostato</t>
         </is>
       </c>
-      <c r="N26" s="38" t="inlineStr"/>
-      <c r="O26" s="36" t="inlineStr"/>
-      <c r="P26" s="38" t="inlineStr"/>
-      <c r="Q26" s="39" t="inlineStr"/>
-      <c r="R26" s="36" t="inlineStr"/>
-      <c r="S26" s="36" t="inlineStr"/>
-      <c r="T26" s="36" t="inlineStr"/>
-      <c r="U26" s="36" t="inlineStr"/>
-      <c r="V26" s="36" t="inlineStr"/>
-      <c r="W26" s="36" t="inlineStr"/>
-      <c r="X26" s="38" t="inlineStr"/>
-      <c r="Y26" s="38" t="inlineStr"/>
-      <c r="Z26" s="40" t="inlineStr"/>
-      <c r="AA26" s="38" t="inlineStr"/>
-      <c r="AB26" s="36" t="inlineStr"/>
-      <c r="AC26" s="36" t="inlineStr"/>
-      <c r="AD26" s="38" t="inlineStr"/>
-      <c r="AE26" s="38" t="inlineStr"/>
-      <c r="AF26" s="38" t="inlineStr"/>
-      <c r="AG26" s="36" t="inlineStr"/>
-      <c r="AH26" s="41" t="inlineStr"/>
+      <c r="N26" s="31" t="inlineStr"/>
+      <c r="O26" s="29" t="inlineStr"/>
+      <c r="P26" s="31" t="inlineStr"/>
+      <c r="Q26" s="32" t="inlineStr"/>
+      <c r="R26" s="29" t="inlineStr"/>
+      <c r="S26" s="29" t="inlineStr"/>
+      <c r="T26" s="29" t="inlineStr"/>
+      <c r="U26" s="29" t="inlineStr"/>
+      <c r="V26" s="29" t="inlineStr"/>
+      <c r="W26" s="29" t="inlineStr"/>
+      <c r="X26" s="31" t="inlineStr"/>
+      <c r="Y26" s="31" t="inlineStr"/>
+      <c r="Z26" s="33" t="inlineStr"/>
+      <c r="AA26" s="31" t="inlineStr"/>
+      <c r="AB26" s="29" t="inlineStr"/>
+      <c r="AC26" s="29" t="inlineStr"/>
+      <c r="AD26" s="31" t="inlineStr"/>
+      <c r="AE26" s="31" t="inlineStr"/>
+      <c r="AF26" s="31" t="inlineStr"/>
+      <c r="AG26" s="29" t="inlineStr"/>
+      <c r="AH26" s="34" t="inlineStr"/>
     </row>
     <row r="27" ht="14.4" customHeight="1">
       <c r="A27" s="8" t="n">
@@ -2898,58 +2893,58 @@
       <c r="AH39" s="20" t="n"/>
     </row>
     <row r="40" ht="14.4" customHeight="1">
-      <c r="A40" s="29" t="n">
+      <c r="A40" s="35" t="n">
         <v>39</v>
       </c>
-      <c r="B40" s="29" t="inlineStr">
+      <c r="B40" s="35" t="inlineStr">
         <is>
           <t>XV</t>
         </is>
       </c>
-      <c r="C40" s="29" t="inlineStr">
+      <c r="C40" s="35" t="inlineStr">
         <is>
           <t>852</t>
         </is>
       </c>
-      <c r="D40" s="29" t="inlineStr"/>
-      <c r="E40" s="30" t="inlineStr">
+      <c r="D40" s="35" t="inlineStr"/>
+      <c r="E40" s="36" t="inlineStr">
         <is>
           <t>XV852</t>
         </is>
       </c>
-      <c r="F40" s="29" t="inlineStr"/>
-      <c r="G40" s="29" t="inlineStr"/>
-      <c r="H40" s="29" t="inlineStr"/>
-      <c r="I40" s="29" t="inlineStr"/>
-      <c r="J40" s="29" t="inlineStr"/>
-      <c r="K40" s="29" t="inlineStr"/>
-      <c r="L40" s="29" t="inlineStr"/>
-      <c r="M40" s="32" t="inlineStr">
+      <c r="F40" s="35" t="inlineStr"/>
+      <c r="G40" s="35" t="inlineStr"/>
+      <c r="H40" s="35" t="inlineStr"/>
+      <c r="I40" s="35" t="inlineStr"/>
+      <c r="J40" s="35" t="inlineStr"/>
+      <c r="K40" s="35" t="inlineStr"/>
+      <c r="L40" s="35" t="inlineStr"/>
+      <c r="M40" s="37" t="inlineStr">
         <is>
           <t>Ball Valve with Pneumatic actuator</t>
         </is>
       </c>
-      <c r="N40" s="32" t="inlineStr"/>
-      <c r="O40" s="29" t="inlineStr"/>
-      <c r="P40" s="32" t="inlineStr"/>
-      <c r="Q40" s="33" t="inlineStr"/>
-      <c r="R40" s="29" t="inlineStr"/>
-      <c r="S40" s="29" t="inlineStr"/>
-      <c r="T40" s="29" t="inlineStr"/>
-      <c r="U40" s="29" t="inlineStr"/>
-      <c r="V40" s="29" t="inlineStr"/>
-      <c r="W40" s="29" t="inlineStr"/>
-      <c r="X40" s="32" t="inlineStr"/>
-      <c r="Y40" s="32" t="inlineStr"/>
-      <c r="Z40" s="34" t="inlineStr"/>
-      <c r="AA40" s="32" t="inlineStr"/>
-      <c r="AB40" s="29" t="inlineStr"/>
-      <c r="AC40" s="29" t="inlineStr"/>
-      <c r="AD40" s="32" t="inlineStr"/>
-      <c r="AE40" s="32" t="inlineStr"/>
-      <c r="AF40" s="32" t="inlineStr"/>
-      <c r="AG40" s="29" t="inlineStr"/>
-      <c r="AH40" s="35" t="inlineStr"/>
+      <c r="N40" s="37" t="inlineStr"/>
+      <c r="O40" s="35" t="inlineStr"/>
+      <c r="P40" s="37" t="inlineStr"/>
+      <c r="Q40" s="38" t="inlineStr"/>
+      <c r="R40" s="35" t="inlineStr"/>
+      <c r="S40" s="35" t="inlineStr"/>
+      <c r="T40" s="35" t="inlineStr"/>
+      <c r="U40" s="35" t="inlineStr"/>
+      <c r="V40" s="35" t="inlineStr"/>
+      <c r="W40" s="35" t="inlineStr"/>
+      <c r="X40" s="37" t="inlineStr"/>
+      <c r="Y40" s="37" t="inlineStr"/>
+      <c r="Z40" s="39" t="inlineStr"/>
+      <c r="AA40" s="37" t="inlineStr"/>
+      <c r="AB40" s="35" t="inlineStr"/>
+      <c r="AC40" s="35" t="inlineStr"/>
+      <c r="AD40" s="37" t="inlineStr"/>
+      <c r="AE40" s="37" t="inlineStr"/>
+      <c r="AF40" s="37" t="inlineStr"/>
+      <c r="AG40" s="35" t="inlineStr"/>
+      <c r="AH40" s="40" t="inlineStr"/>
     </row>
     <row r="41" ht="14.4" customHeight="1">
       <c r="A41" s="8" t="n"/>

</xml_diff>